<commit_message>
Discard invalid ipv4 ips, inswtich
</commit_message>
<xml_diff>
--- a/docs/mlaas_preli/result.xlsx
+++ b/docs/mlaas_preli/result.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95346063eca47658/documents/computerScience/RIT/2023 spring/NetworkingResearch/inswitch_anomaly/docs/mlaas_preli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_F25DC773A252ABDACC104860D19C425A5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4578937E-5B28-42A7-8940-02AA271317E2}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC104860D19C425A5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84DB23C7-A5BB-4EB6-BA59-A0FE623E9ED2}"/>
   <bookViews>
-    <workbookView xWindow="456" yWindow="3168" windowWidth="17280" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3084" yWindow="2700" windowWidth="17280" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,6 +22,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>local test</t>
+  </si>
+  <si>
+    <t>one client, one switch</t>
+  </si>
+  <si>
+    <t>two clients, one switch</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,15 +355,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0.67447918653488104</v>
       </c>
@@ -360,8 +373,11 @@
       <c r="C1">
         <v>0.68489581346511796</v>
       </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.66015625</v>
       </c>
@@ -371,30 +387,21 @@
       <c r="C2">
         <v>0.69010418653488104</v>
       </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8C74A2-F981-4144-9E65-C4CFE3BE63A8}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>0.71614581346511796</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0.67057293853488098</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0.65104168653488104</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.65625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Balanced reformatted dataset, ptf test.
</commit_message>
<xml_diff>
--- a/docs/mlaas_preli/result.xlsx
+++ b/docs/mlaas_preli/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95346063eca47658/documents/computerScience/RIT/2023 spring/NetworkingResearch/inswitch_anomaly/docs/mlaas_preli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC104860D19C425A5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84DB23C7-A5BB-4EB6-BA59-A0FE623E9ED2}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_F25DC773A252ABDACC104860D19C425A5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{150F1BFA-0360-40C9-9A1D-5AE267215EC2}"/>
   <bookViews>
-    <workbookView xWindow="3084" yWindow="2700" windowWidth="17280" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19485" yWindow="9255" windowWidth="17250" windowHeight="10485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -358,12 +358,12 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0.67447918653488104</v>
       </c>
@@ -377,7 +377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.66015625</v>
       </c>
@@ -391,17 +391,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.67057293853488098</v>
       </c>
+      <c r="B4">
+        <v>0.65234749999999997</v>
+      </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.65625</v>
+      </c>
+      <c r="B5">
+        <v>0.69791668653488104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bugs in producing trees and mapping process.
</commit_message>
<xml_diff>
--- a/docs/mlaas_preli/result.xlsx
+++ b/docs/mlaas_preli/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95346063eca47658/documents/computerScience/RIT/2023 spring/NetworkingResearch/inswitch_anomaly/docs/mlaas_preli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_F25DC773A252ABDACC104860D19C425A5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{150F1BFA-0360-40C9-9A1D-5AE267215EC2}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_F25DC773A252ABDACC104860D19C425A5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{802F5A6F-26F8-4EBB-8B58-B78DBA091223}"/>
   <bookViews>
-    <workbookView xWindow="19485" yWindow="9255" windowWidth="17250" windowHeight="10485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5508" yWindow="8640" windowWidth="15672" windowHeight="5604" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,10 +86,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -355,15 +351,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0.67447918653488104</v>
       </c>
@@ -377,7 +373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.66015625</v>
       </c>
@@ -391,7 +387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.67057293853488098</v>
       </c>
@@ -402,12 +398,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.65625</v>
       </c>
       <c r="B5">
         <v>0.69791668653488104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.64453125</v>
+      </c>
+      <c r="B6">
+        <v>0.68619793653488104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified sketching pseudocode and code comments.
</commit_message>
<xml_diff>
--- a/docs/mlaas_preli/result.xlsx
+++ b/docs/mlaas_preli/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95346063eca47658/documents/computerScience/RIT/2023 spring/NetworkingResearch/inswitch_anomaly/docs/mlaas_preli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="11_F25DC773A252ABDACC104860D19C425A5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B22701B3-D4F8-400F-BFC4-8211EABF4281}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="11_F25DC773A252ABDACC104860D19C425A5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{096A7A93-417F-43EE-B1CE-2780FB4E56DE}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="10548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>local test</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>two clients, one switch, bmv2</t>
+  </si>
+  <si>
+    <t>one client, one switch, tofino</t>
+  </si>
+  <si>
+    <t>two clients, one switch, tofino</t>
   </si>
 </sst>
 </file>
@@ -106,6 +112,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,15 +381,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0.67447918653488104</v>
       </c>
@@ -397,7 +407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.66015625</v>
       </c>
@@ -423,8 +433,15 @@
       <c r="L2">
         <v>0.68359375</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2" s="1">
+        <f>AVERAGE(J2:L2)</f>
+        <v>0.69444443782170595</v>
+      </c>
+      <c r="O2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.67057293853488098</v>
       </c>
@@ -434,8 +451,17 @@
       <c r="F4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <v>0.67838543653488104</v>
+      </c>
+      <c r="K4">
+        <v>0.66145831346511796</v>
+      </c>
+      <c r="O4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.65625</v>
       </c>
@@ -443,7 +469,7 @@
         <v>0.69791668653488104</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.64453125</v>
       </c>
@@ -451,7 +477,7 @@
         <v>0.68619793653488104</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f>AVERAGE(A4:A6)</f>
         <v>0.65711806284496033</v>

</xml_diff>